<commit_message>
tg: update sch sth forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Togo/2023/tg_sch_sth_impact_202309_2_child.xlsx
+++ b/SCH-STH/Impact assessments/Togo/2023/tg_sch_sth_impact_202309_2_child.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Togo\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33539AD-1409-49BB-8435-E32EAB6A439C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B3655C-0738-4A62-B826-CA42EA3A89F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="187">
   <si>
     <t>type</t>
   </si>
@@ -503,12 +503,6 @@
     <t>French</t>
   </si>
   <si>
-    <t>regex(.,'^[a-zA-Z]{2,4}$')</t>
-  </si>
-  <si>
-    <t>Doit contenir 2 à 4 caractère alphanumérique</t>
-  </si>
-  <si>
     <t>p_usp</t>
   </si>
   <si>
@@ -584,9 +578,6 @@
     <t>MONTANT Minyo Ega Sossa</t>
   </si>
   <si>
-    <t>N’DATO Kossi</t>
-  </si>
-  <si>
     <t xml:space="preserve">NAKOME Bamouni </t>
   </si>
   <si>
@@ -645,6 +636,9 @@
   </si>
   <si>
     <t>select_one recorders</t>
+  </si>
+  <si>
+    <t>NDATO Kossi</t>
   </si>
 </sst>
 </file>
@@ -1152,7 +1146,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1209,9 +1203,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="5" customFormat="1" ht="31.5">
+    <row r="2" spans="1:12" s="5" customFormat="1">
       <c r="A2" s="31" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>12</v>
@@ -1221,12 +1215,8 @@
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="9"/>
-      <c r="F2" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>142</v>
-      </c>
+      <c r="F2" s="26"/>
+      <c r="G2" s="27"/>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9" t="s">
@@ -1240,10 +1230,10 @@
         <v>15</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="8"/>
@@ -1284,7 +1274,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>18</v>
@@ -1324,7 +1314,7 @@
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="17" customFormat="1" ht="169.5" customHeight="1">
@@ -1384,10 +1374,10 @@
       <c r="D9" s="10"/>
       <c r="E9" s="9"/>
       <c r="F9" s="26" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G9" s="30" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>32</v>
@@ -1402,18 +1392,18 @@
         <v>29</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="9"/>
       <c r="F10" s="26" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>32</v>
@@ -1683,7 +1673,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1721,10 +1711,10 @@
         <v>72</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="15"/>
@@ -1736,10 +1726,10 @@
         <v>72</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="15"/>
@@ -1751,10 +1741,10 @@
         <v>72</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="15"/>
@@ -1766,10 +1756,10 @@
         <v>72</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="15"/>
@@ -1781,10 +1771,10 @@
         <v>72</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="15"/>
@@ -1796,10 +1786,10 @@
         <v>72</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="15"/>
@@ -1811,10 +1801,10 @@
         <v>72</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="15"/>
@@ -1826,10 +1816,10 @@
         <v>72</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="15"/>
@@ -1841,10 +1831,10 @@
         <v>72</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="15"/>
@@ -1856,10 +1846,10 @@
         <v>72</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="15"/>
@@ -1871,10 +1861,10 @@
         <v>72</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="15"/>
@@ -1886,10 +1876,10 @@
         <v>72</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="15"/>
@@ -1901,10 +1891,10 @@
         <v>72</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="15"/>
@@ -1916,10 +1906,10 @@
         <v>72</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="15"/>
@@ -1931,10 +1921,10 @@
         <v>72</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="15"/>
@@ -1946,10 +1936,10 @@
         <v>72</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="15"/>
@@ -1961,10 +1951,10 @@
         <v>72</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="15"/>
@@ -1976,10 +1966,10 @@
         <v>72</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="15"/>
@@ -1991,10 +1981,10 @@
         <v>72</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="15"/>
@@ -2021,10 +2011,10 @@
         <v>72</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="15"/>
@@ -2036,10 +2026,10 @@
         <v>72</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="15"/>
@@ -2051,10 +2041,10 @@
         <v>72</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="15"/>
@@ -2066,10 +2056,10 @@
         <v>72</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D25" s="28"/>
       <c r="E25" s="29"/>
@@ -2081,10 +2071,10 @@
         <v>72</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="D26" s="28"/>
       <c r="E26" s="29"/>
@@ -2096,10 +2086,10 @@
         <v>72</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D27" s="28"/>
       <c r="E27" s="29"/>
@@ -2126,10 +2116,10 @@
         <v>72</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D29" s="28"/>
       <c r="E29" s="29"/>
@@ -2141,10 +2131,10 @@
         <v>72</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D30" s="28"/>
       <c r="E30" s="29"/>
@@ -2156,10 +2146,10 @@
         <v>72</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D31" s="28"/>
       <c r="E31" s="29"/>
@@ -2171,10 +2161,10 @@
         <v>72</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D32" s="28"/>
       <c r="E32" s="29"/>
@@ -2201,10 +2191,10 @@
         <v>72</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D34" s="28"/>
       <c r="E34" s="29"/>
@@ -2216,10 +2206,10 @@
         <v>72</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D35" s="28"/>
       <c r="E35" s="29"/>
@@ -2231,10 +2221,10 @@
         <v>72</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D36" s="28"/>
       <c r="E36" s="29"/>
@@ -2246,10 +2236,10 @@
         <v>72</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D37" s="28"/>
       <c r="E37" s="29"/>
@@ -4710,10 +4700,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C2" t="s">
         <v>140</v>

</xml_diff>

<commit_message>
tg: update some forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Togo/2023/tg_sch_sth_impact_202309_2_child.xlsx
+++ b/SCH-STH/Impact assessments/Togo/2023/tg_sch_sth_impact_202309_2_child.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Togo\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8214D843-6E44-4384-A76E-0288D0A398E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347026B3-A2A5-4C94-BF34-998566DDF0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="191">
   <si>
     <t>type</t>
   </si>
@@ -299,12 +299,6 @@
     <t>HOUNYOVI Ayaovi</t>
   </si>
   <si>
-    <t>NOUSSOUGNON Kokou</t>
-  </si>
-  <si>
-    <t>SOH Atafembou</t>
-  </si>
-  <si>
     <t>yesNo</t>
   </si>
   <si>
@@ -467,12 +461,6 @@
     <t>Négatif</t>
   </si>
   <si>
-    <t>Trace.non.hemolysee</t>
-  </si>
-  <si>
-    <t>Trace non hémolysée</t>
-  </si>
-  <si>
     <t>Trace.hemolysee</t>
   </si>
   <si>
@@ -506,30 +494,18 @@
     <t>subdistrict_list= ${p_usp}</t>
   </si>
   <si>
-    <t>ABAYE Elom</t>
-  </si>
-  <si>
     <t>ABDOU-KERIM Agueregna</t>
   </si>
   <si>
-    <t>ADABRA Hélène</t>
-  </si>
-  <si>
     <t>ADJAGODO Gadiel</t>
   </si>
   <si>
-    <t>ADJENDA Eke</t>
-  </si>
-  <si>
     <t>AFANOU Kokou M</t>
   </si>
   <si>
     <t>AGBOZO Senyo</t>
   </si>
   <si>
-    <t>AKOBI  Komi</t>
-  </si>
-  <si>
     <t>AKUTSA Kafui</t>
   </si>
   <si>
@@ -539,66 +515,33 @@
     <t>BADJASSEM Gloria Diyane</t>
   </si>
   <si>
-    <t>BAKOLTINA Disrama Denise</t>
-  </si>
-  <si>
     <t>BATEBAWI Raphaël</t>
   </si>
   <si>
-    <t>DJAMAH Prosper</t>
-  </si>
-  <si>
-    <t>DJOBO Annissah</t>
-  </si>
-  <si>
     <t>DOUMONGUE Tibanguebé</t>
   </si>
   <si>
     <t>EKAHOHO Yaovi</t>
   </si>
   <si>
-    <t>GBOGBATSE Komi Mensa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GNANLABA Pyabalo </t>
-  </si>
-  <si>
     <t>KOKAN Faïzat</t>
   </si>
   <si>
     <t>KUTOATI Abla</t>
   </si>
   <si>
-    <t xml:space="preserve">LOGO Kokou </t>
-  </si>
-  <si>
     <t>MONTANT Minyo Ega Sossa</t>
   </si>
   <si>
-    <t xml:space="preserve">NAKOME Bamouni </t>
-  </si>
-  <si>
-    <t>PORO Kpatcha Edjareguew</t>
-  </si>
-  <si>
     <t>SAGOA Djamsa</t>
   </si>
   <si>
-    <t>SEDJRO Afantolo</t>
-  </si>
-  <si>
-    <t>SINGO ATTAH</t>
-  </si>
-  <si>
     <t>SOLI Lontassam</t>
   </si>
   <si>
     <t>SOTOU Novinyo</t>
   </si>
   <si>
-    <t>TAGBA Atna Edi</t>
-  </si>
-  <si>
     <t>TCHAGBELE Wanikougnon</t>
   </si>
   <si>
@@ -623,43 +566,91 @@
     <t>select_one recorders</t>
   </si>
   <si>
-    <t>NDATO Kossi</t>
-  </si>
-  <si>
     <t>Le résultat est positif, l'urine doit être conservé.</t>
   </si>
   <si>
     <t>if((${p_grading} = '+' or ${p_grading} = '++' or ${p_grading} = '+++' or ${p_grading} = 'Trace.hemolysee'), . = 'Oui', true())</t>
   </si>
   <si>
-    <t>(2023 Sept) - 2. SCH/STH – Enrôlement V3</t>
-  </si>
-  <si>
-    <t>tg_sch_sth_impact_202309_2_child_v3</t>
-  </si>
-  <si>
-    <t>select_one yesNo</t>
-  </si>
-  <si>
-    <t>p_control</t>
-  </si>
-  <si>
-    <t>La bandelette est-elle retenue pour le contrôle qualité</t>
-  </si>
-  <si>
-    <t>p_grading2</t>
-  </si>
-  <si>
-    <t>Contrôle de Graduation de la microhématurie</t>
-  </si>
-  <si>
-    <t>${p_consent} = 'A.donne'  and ${p_collected_urine} = 'Oui' and ${p_control} = 'Oui'</t>
-  </si>
-  <si>
     <t xml:space="preserve">L'urine  est-elle conservée pour la filtration de l’urine? </t>
   </si>
   <si>
     <t>Il s'agit de l'urine de bandellete et/ou de l'urine macroscopiquement positive.</t>
+  </si>
+  <si>
+    <t>tg_sch_sth_impact_202309_2_child_v4</t>
+  </si>
+  <si>
+    <t>(2023 Sept) - 2. SCH/STH – Enrôlement V4</t>
+  </si>
+  <si>
+    <t>L’urine est-elle macroscopiquement hématurique</t>
+  </si>
+  <si>
+    <t>p_macroscopique_hemat</t>
+  </si>
+  <si>
+    <t>ABAYE Kokou Mawulom</t>
+  </si>
+  <si>
+    <t>ADABRA Abra Hélène</t>
+  </si>
+  <si>
+    <t>ADJINDA Eké</t>
+  </si>
+  <si>
+    <t>AKOBI Komi</t>
+  </si>
+  <si>
+    <t>BAKOLITANA Disrama Denise</t>
+  </si>
+  <si>
+    <t>DJAMAH Yaovi Prosper</t>
+  </si>
+  <si>
+    <t>DJOBO Anissah</t>
+  </si>
+  <si>
+    <t>FONVI Akakpo</t>
+  </si>
+  <si>
+    <t>GBOGBATSE</t>
+  </si>
+  <si>
+    <t>GNANLABA Pyabalo</t>
+  </si>
+  <si>
+    <t>LACK Fiali,</t>
+  </si>
+  <si>
+    <t>LOGO Kokou Dodji</t>
+  </si>
+  <si>
+    <t>N’DATO Kossi</t>
+  </si>
+  <si>
+    <t>NAKOME Bamouni</t>
+  </si>
+  <si>
+    <t>NOUSSOUGNON Kokou S.</t>
+  </si>
+  <si>
+    <t>PORO Kpatcha Edjaréguéw</t>
+  </si>
+  <si>
+    <t>SEDJRO Afantolou</t>
+  </si>
+  <si>
+    <t>SINGO Kodjo ATTAH</t>
+  </si>
+  <si>
+    <t>SOH Aféyibou</t>
+  </si>
+  <si>
+    <t>TAGBA Atna-Edi M.</t>
+  </si>
+  <si>
+    <t>YAKPA Kossi</t>
   </si>
 </sst>
 </file>
@@ -733,7 +724,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -756,12 +747,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFFFF"/>
         <bgColor rgb="FFCCFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFFF"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -833,7 +818,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -916,22 +901,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1208,13 +1177,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A16" sqref="A16:XFD16"/>
+      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1273,7 +1242,7 @@
     </row>
     <row r="2" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>12</v>
@@ -1320,7 +1289,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>18</v>
@@ -1360,7 +1329,7 @@
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="8" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="17" customFormat="1" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1420,10 +1389,10 @@
       <c r="D8" s="10"/>
       <c r="E8" s="9"/>
       <c r="F8" s="26" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>32</v>
@@ -1438,18 +1407,18 @@
         <v>29</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="9"/>
       <c r="F9" s="26" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>32</v>
@@ -1565,13 +1534,13 @@
     </row>
     <row r="14" spans="1:12" s="17" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>49</v>
+        <v>33</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>169</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>50</v>
+        <v>168</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="8"/>
@@ -1585,27 +1554,27 @@
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
     </row>
-    <row r="15" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
-        <v>186</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>188</v>
-      </c>
-      <c r="D15" s="35"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
+    <row r="15" spans="1:12" s="17" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I15" s="8"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
     </row>
     <row r="16" spans="1:12" s="17" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
@@ -1615,17 +1584,17 @@
         <v>52</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>53</v>
@@ -1637,69 +1606,65 @@
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
     </row>
-    <row r="17" spans="1:12" s="17" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>189</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>190</v>
-      </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="26" t="s">
-        <v>191</v>
-      </c>
-      <c r="I17" s="8"/>
-      <c r="J17" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-    </row>
-    <row r="18" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+    </row>
+    <row r="18" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="12"/>
       <c r="H18" s="8" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
       <c r="K18" s="11"/>
       <c r="L18" s="11"/>
     </row>
-    <row r="19" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="12"/>
-      <c r="H19" s="8" t="s">
-        <v>59</v>
-      </c>
+      <c r="H19" s="8"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
       <c r="K19" s="11"/>
@@ -1707,14 +1672,12 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>61</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C20" s="22"/>
       <c r="D20" s="12"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
@@ -1726,11 +1689,11 @@
       <c r="L20" s="11"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>62</v>
+      <c r="A21" s="9" t="s">
+        <v>64</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="12"/>
@@ -1743,37 +1706,19 @@
       <c r="K21" s="11"/>
       <c r="L21" s="11"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G479"/>
+  <dimension ref="A1:G481"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1811,10 +1756,10 @@
         <v>71</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="15"/>
@@ -1826,10 +1771,10 @@
         <v>71</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="15"/>
@@ -1841,10 +1786,10 @@
         <v>71</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="15"/>
@@ -1856,10 +1801,10 @@
         <v>71</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="15"/>
@@ -1871,10 +1816,10 @@
         <v>71</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>146</v>
+        <v>172</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>146</v>
+        <v>172</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="15"/>
@@ -1886,10 +1831,10 @@
         <v>71</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="15"/>
@@ -1901,10 +1846,10 @@
         <v>71</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="15"/>
@@ -1916,10 +1861,10 @@
         <v>71</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="15"/>
@@ -1931,10 +1876,10 @@
         <v>71</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="15"/>
@@ -1946,10 +1891,10 @@
         <v>71</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="15"/>
@@ -1961,10 +1906,10 @@
         <v>71</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="15"/>
@@ -1976,10 +1921,10 @@
         <v>71</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="15"/>
@@ -1991,10 +1936,10 @@
         <v>71</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="15"/>
@@ -2006,10 +1951,10 @@
         <v>71</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="15"/>
@@ -2021,10 +1966,10 @@
         <v>71</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="15"/>
@@ -2036,10 +1981,10 @@
         <v>71</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="15"/>
@@ -2051,10 +1996,10 @@
         <v>71</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="15"/>
@@ -2066,10 +2011,10 @@
         <v>71</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="15"/>
@@ -2081,10 +2026,10 @@
         <v>71</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="15"/>
@@ -2096,10 +2041,10 @@
         <v>71</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>72</v>
+        <v>179</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>72</v>
+        <v>179</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="15"/>
@@ -2111,10 +2056,10 @@
         <v>71</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="15"/>
@@ -2126,10 +2071,10 @@
         <v>71</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="15"/>
@@ -2141,10 +2086,10 @@
         <v>71</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="15"/>
@@ -2156,10 +2101,10 @@
         <v>71</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
       <c r="D25" s="28"/>
       <c r="E25" s="29"/>
@@ -2186,10 +2131,10 @@
         <v>71</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="D27" s="28"/>
       <c r="E27" s="29"/>
@@ -2201,10 +2146,10 @@
         <v>71</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>73</v>
+        <v>182</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>73</v>
+        <v>182</v>
       </c>
       <c r="D28" s="28"/>
       <c r="E28" s="29"/>
@@ -2216,10 +2161,10 @@
         <v>71</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
       <c r="D29" s="28"/>
       <c r="E29" s="29"/>
@@ -2231,10 +2176,10 @@
         <v>71</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="D30" s="28"/>
       <c r="E30" s="29"/>
@@ -2246,10 +2191,10 @@
         <v>71</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="D31" s="28"/>
       <c r="E31" s="29"/>
@@ -2261,10 +2206,10 @@
         <v>71</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="D32" s="28"/>
       <c r="E32" s="29"/>
@@ -2276,10 +2221,10 @@
         <v>71</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>74</v>
+        <v>186</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>74</v>
+        <v>186</v>
       </c>
       <c r="D33" s="28"/>
       <c r="E33" s="29"/>
@@ -2291,10 +2236,10 @@
         <v>71</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="D34" s="28"/>
       <c r="E34" s="29"/>
@@ -2306,10 +2251,10 @@
         <v>71</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="D35" s="28"/>
       <c r="E35" s="29"/>
@@ -2321,10 +2266,10 @@
         <v>71</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="D36" s="28"/>
       <c r="E36" s="29"/>
@@ -2336,10 +2281,10 @@
         <v>71</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="D37" s="28"/>
       <c r="E37" s="29"/>
@@ -2347,395 +2292,415 @@
       <c r="G37" s="16"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
+      <c r="A38" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>189</v>
+      </c>
       <c r="D38" s="28"/>
       <c r="E38" s="29"/>
       <c r="F38" s="16"/>
       <c r="G38" s="16"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
-        <v>75</v>
+      <c r="A39" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>76</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D39" s="28"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
-        <v>75</v>
+      <c r="A40" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>77</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D40" s="28"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="9"/>
+      <c r="A41" s="8"/>
       <c r="B41" s="9"/>
-      <c r="C41" s="10"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="10"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B46" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>87</v>
+      <c r="C46" s="13" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C49" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B62" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B62" s="9" t="s">
-        <v>117</v>
-      </c>
       <c r="C62" s="10" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B64" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B68" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C64" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="14" t="s">
+      <c r="C68" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B65" s="5" t="s">
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B69" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C69" s="5" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>126</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>126</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>126</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>124</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C70" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="B70" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="C70" s="24" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>126</v>
-      </c>
-      <c r="B71" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="C71" s="24" t="s">
-        <v>134</v>
+        <v>124</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B72" s="24" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C72" s="24" t="s">
-        <v>135</v>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>124</v>
+      </c>
+      <c r="B73" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="C73" s="24" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="11"/>
-      <c r="B74" s="4"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
-      <c r="E74" s="15"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="11"/>
-      <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="15"/>
+      <c r="A74" t="s">
+        <v>124</v>
+      </c>
+      <c r="B74" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C74" s="24" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="11"/>
@@ -2794,18 +2759,22 @@
       <c r="E83" s="15"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B84"/>
-      <c r="C84"/>
+      <c r="A84" s="11"/>
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="15"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="11"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
-      <c r="E85" s="4"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="15"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B86" s="4"/>
-      <c r="C86" s="4"/>
-      <c r="E86" s="4"/>
+      <c r="B86"/>
+      <c r="C86"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B87" s="4"/>
@@ -3257,15 +3226,15 @@
       <c r="C176" s="4"/>
       <c r="E176" s="4"/>
     </row>
+    <row r="177" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B177" s="4"/>
+      <c r="C177" s="4"/>
+      <c r="E177" s="4"/>
+    </row>
     <row r="178" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B178" s="4"/>
       <c r="C178" s="4"/>
-      <c r="F178" s="4"/>
-    </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B179" s="4"/>
-      <c r="C179" s="4"/>
-      <c r="F179" s="4"/>
+      <c r="E178" s="4"/>
     </row>
     <row r="180" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B180" s="4"/>
@@ -4766,6 +4735,16 @@
       <c r="B479" s="4"/>
       <c r="C479" s="4"/>
       <c r="F479" s="4"/>
+    </row>
+    <row r="480" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B480" s="4"/>
+      <c r="C480" s="4"/>
+      <c r="F480" s="4"/>
+    </row>
+    <row r="481" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B481" s="4"/>
+      <c r="C481" s="4"/>
+      <c r="F481" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -4778,7 +4757,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4789,24 +4768,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="C2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tg: improve sch/sth forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Togo/2023/tg_sch_sth_impact_202309_2_child.xlsx
+++ b/SCH-STH/Impact assessments/Togo/2023/tg_sch_sth_impact_202309_2_child.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Togo\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED79683A-85D0-481D-97AB-E487D7AE2953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42894114-F6B0-4EC5-805E-0052DD49F4C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -638,19 +638,19 @@
     <t>YAKPA Kossi</t>
   </si>
   <si>
-    <t>(2023 Sept) - 2. SCH/STH – Enrôlement V4.1</t>
-  </si>
-  <si>
-    <t>tg_sch_sth_impact_202309_2_child_v4_1</t>
-  </si>
-  <si>
-    <t>if((${p_grading} = 'Negatif' and ${p_macroscopique_hemat} = 'Non'), . = 'Oui', true())</t>
-  </si>
-  <si>
-    <t>L'urine doit être conservé parce que macroscopiquement  négative  et de graduation  négative</t>
-  </si>
-  <si>
-    <t>${p_consent} = 'A.donne' and ${p_collected_urine} = 'Oui' and ${p_grading} = 'Negatif' and ${p_macroscopique_hemat} = 'Non'</t>
+    <t>(2023 Sept) - 2. SCH/STH – Enrôlement V4.2</t>
+  </si>
+  <si>
+    <t>tg_sch_sth_impact_202309_2_child_v4_2</t>
+  </si>
+  <si>
+    <t>L'urine doit être conservé parce que macroscopiquement  positive  et de graduation  positive</t>
+  </si>
+  <si>
+    <t>if((${p_grading} = '+' or ${p_grading} = '++' or ${p_grading} = '+++' or ${p_grading} = 'Trace.hemolysee' or  ${p_macroscopique_hemat} = 'Oui'), . = 'Oui', true())</t>
+  </si>
+  <si>
+    <t>${p_consent} = 'A.donne' and ${p_collected_urine} = 'Oui' and (${p_grading} = '+' or ${p_grading} = '++' or ${p_grading} = '+++' or ${p_grading} = 'Trace.hemolysee' or ${p_macroscopique_hemat} = 'Oui')</t>
   </si>
 </sst>
 </file>
@@ -1183,7 +1183,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1576,7 +1576,7 @@
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
     </row>
-    <row r="16" spans="1:12" s="17" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" s="17" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>33</v>
       </c>
@@ -1591,10 +1591,10 @@
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="G16" s="23" t="s">
         <v>188</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>189</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>190</v>
@@ -1718,7 +1718,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B70" sqref="B70"/>
+      <selection pane="bottomLeft" activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4757,7 +4757,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>